<commit_message>
Administration et Portail web diagrammes des exigences
</commit_message>
<xml_diff>
--- a/documentation/diagrammes/dal/table_export.xls.xlsx
+++ b/documentation/diagrammes/dal/table_export.xls.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv-my.sharepoint.com/personal/samer_machara-marquez_esante_gouv_fr/Documents/Documents/projets/finess-plus/documentation/diagrammes/dal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:4000b_{AA23CF93-0DD1-4124-8A91-A936038E3C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:4000b_{AA23CF93-0DD1-4124-8A91-A936038E3C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99A38900-0C3E-4F13-929C-ECFC706BE166}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$47</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -426,7 +429,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1314,11 +1317,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1338,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="132" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="132" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1349,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="115.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="115.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1393,7 +1397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="132" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="132" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="33" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1415,7 +1419,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="99" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="99" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1426,7 +1430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1437,7 +1441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1459,7 +1463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1468,7 +1472,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="82.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1479,7 +1483,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1490,7 +1494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="148.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="148.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
@@ -1501,7 +1505,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="82.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1512,7 +1516,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
@@ -1523,7 +1527,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -1545,7 +1549,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="82.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
@@ -1567,7 +1571,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
@@ -1578,7 +1582,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="82.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>67</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>70</v>
       </c>
@@ -1600,7 +1604,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>73</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="99" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="99" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -1622,7 +1626,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="115.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="115.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -1633,7 +1637,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="99" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="99" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="132" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="132" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
@@ -1655,7 +1659,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="66" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>88</v>
       </c>
@@ -1666,7 +1670,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="99" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="99" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>91</v>
       </c>
@@ -1677,7 +1681,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="99" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="99" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>94</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="82.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>97</v>
       </c>
@@ -1699,7 +1703,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
@@ -1710,7 +1714,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="49.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>103</v>
       </c>
@@ -1721,7 +1725,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="82.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>106</v>
       </c>
@@ -1837,13 +1841,29 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C47" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="REQ-2.4.3 Synchronisation en lot"/>
+        <filter val="REQ-2.4.3.1 Configuration du format d'entrée"/>
+        <filter val="REQ-2.4.3.2 Compatibilité des formats"/>
+        <filter val="REQ-2.4.3.3 Configuration du format de sortie"/>
+        <filter val="REQ-2.4.3.4 Mappage des données"/>
+        <filter val="REQ-2.4.3.5 Gestion des erreurs"/>
+        <filter val="REQ-2.4.3.5 Notification des erreurs"/>
+        <filter val="REQ-2.4.3.6 Surveillance de la synchronisation"/>
+        <filter val="REQ-2.4.3.7 Contrôle des versions"/>
+        <filter val="REQ-2.4.3.8 Validation des données"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1855,7 +1875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>